<commit_message>
Updated student bulk upload functionality
</commit_message>
<xml_diff>
--- a/public/template/student_template.xlsx
+++ b/public/template/student_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <r>
       <rPr>
@@ -56,6 +56,9 @@
     <t>Choudhary</t>
   </si>
   <si>
+    <t>01-01-2000</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -65,31 +68,13 @@
     <t>guardian-1@gmail.com</t>
   </si>
   <si>
-    <t>Ajay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Akash </t>
-  </si>
-  <si>
-    <t>Akshara</t>
-  </si>
-  <si>
-    <t>Jain</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Mr. Ravi Jain</t>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -131,7 +116,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -395,58 +380,27 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3">
-        <v>36526.0</v>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1.23456789E9</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3">
-        <v>36892.0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.345678901E9</v>
-      </c>
+      <c r="I4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>